<commit_message>
avg setting make increment
we  are make change in average for current count
</commit_message>
<xml_diff>
--- a/cureent table.xlsx
+++ b/cureent table.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Embeded file 14_06_19\ms 51 controller_All Programe\PWM_Simple - kunjanbhai current adC\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Embeded file 14_06_19\ms 51 controller_All Programe\smart_switch\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -82,14 +82,14 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="16"/>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="16"/>
+      <sz val="12"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -117,7 +117,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -142,6 +142,8 @@
     <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -425,22 +427,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A6:H66"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="21" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.28515625" style="6" customWidth="1"/>
-    <col min="2" max="3" width="17" style="2" customWidth="1"/>
+    <col min="1" max="1" width="3.140625" style="6" customWidth="1"/>
+    <col min="2" max="2" width="17" style="2" customWidth="1"/>
+    <col min="3" max="3" width="10.85546875" style="2" hidden="1" customWidth="1"/>
     <col min="4" max="4" width="16.28515625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="36.7109375" style="4" customWidth="1"/>
-    <col min="6" max="6" width="37.7109375" style="5" customWidth="1"/>
+    <col min="5" max="5" width="16.7109375" style="4" customWidth="1"/>
+    <col min="6" max="6" width="14.28515625" style="12" customWidth="1"/>
     <col min="7" max="7" width="15" style="5" customWidth="1"/>
     <col min="8" max="16384" width="9.140625" style="6"/>
   </cols>
   <sheetData>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
         <v>6</v>
       </c>
@@ -453,11 +456,11 @@
       <c r="E6" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F6" s="5" t="s">
+      <c r="F6" s="12" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B7" s="2">
         <v>0.5</v>
       </c>
@@ -465,18 +468,18 @@
         <v>0.7</v>
       </c>
       <c r="D7" s="2">
-        <v>0.64</v>
+        <v>0.5</v>
       </c>
       <c r="E7" s="4">
-        <f>B7/D7</f>
-        <v>0.78125</v>
-      </c>
-      <c r="F7" s="5">
-        <f>D7*E7</f>
+        <f t="shared" ref="E7:E35" si="0">B7/D7</f>
+        <v>1</v>
+      </c>
+      <c r="F7" s="12">
+        <f t="shared" ref="F7:F35" si="1">D7*E7</f>
         <v>0.5</v>
       </c>
     </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B8" s="2">
         <v>1</v>
       </c>
@@ -484,18 +487,18 @@
         <v>1.1100000000000001</v>
       </c>
       <c r="D8" s="2">
-        <v>0.94</v>
+        <v>0.99</v>
       </c>
       <c r="E8" s="4">
-        <f>B8/D8</f>
-        <v>1.0638297872340425</v>
-      </c>
-      <c r="F8" s="5">
+        <f t="shared" si="0"/>
+        <v>1.0101010101010102</v>
+      </c>
+      <c r="F8" s="12">
         <f>D8*E8</f>
-        <v>0.99999999999999989</v>
-      </c>
-    </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B9" s="2">
         <v>1.5</v>
       </c>
@@ -503,18 +506,18 @@
         <v>1.61</v>
       </c>
       <c r="D9" s="2">
-        <v>1.41</v>
+        <v>1.32</v>
       </c>
       <c r="E9" s="4">
-        <f>B9/D9</f>
-        <v>1.0638297872340425</v>
-      </c>
-      <c r="F9" s="5">
-        <f>D9*E9</f>
-        <v>1.4999999999999998</v>
-      </c>
-    </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.35">
+        <f t="shared" si="0"/>
+        <v>1.1363636363636362</v>
+      </c>
+      <c r="F9" s="12">
+        <f t="shared" si="1"/>
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B10" s="2">
         <v>2</v>
       </c>
@@ -522,18 +525,18 @@
         <v>2.06</v>
       </c>
       <c r="D10" s="2">
-        <v>1.78</v>
+        <v>1.81</v>
       </c>
       <c r="E10" s="4">
-        <f>B10/D10</f>
-        <v>1.1235955056179776</v>
-      </c>
-      <c r="F10" s="5">
-        <f>D10*E10</f>
+        <f t="shared" si="0"/>
+        <v>1.1049723756906078</v>
+      </c>
+      <c r="F10" s="12">
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B11" s="2">
         <v>2.5</v>
       </c>
@@ -541,18 +544,18 @@
         <v>2.56</v>
       </c>
       <c r="D11" s="2">
-        <v>2.29</v>
+        <v>2.14</v>
       </c>
       <c r="E11" s="4">
-        <f>B11/D11</f>
-        <v>1.0917030567685588</v>
-      </c>
-      <c r="F11" s="5">
-        <f>D11*E11</f>
-        <v>2.4999999999999996</v>
-      </c>
-    </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.35">
+        <f t="shared" si="0"/>
+        <v>1.1682242990654206</v>
+      </c>
+      <c r="F11" s="12">
+        <f t="shared" si="1"/>
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B12" s="2">
         <v>3</v>
       </c>
@@ -560,18 +563,18 @@
         <v>3.01</v>
       </c>
       <c r="D12" s="2">
-        <v>2.66</v>
+        <v>2.63</v>
       </c>
       <c r="E12" s="4">
-        <f>B12/D12</f>
-        <v>1.1278195488721805</v>
-      </c>
-      <c r="F12" s="5">
-        <f>D12*E12</f>
-        <v>3.0000000000000004</v>
-      </c>
-    </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.35">
+        <f t="shared" si="0"/>
+        <v>1.1406844106463878</v>
+      </c>
+      <c r="F12" s="12">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B13" s="2">
         <v>3.5</v>
       </c>
@@ -579,18 +582,18 @@
         <v>3.51</v>
       </c>
       <c r="D13" s="2">
-        <v>3.08</v>
+        <v>3.11</v>
       </c>
       <c r="E13" s="4">
-        <f>B13/D13</f>
-        <v>1.1363636363636362</v>
-      </c>
-      <c r="F13" s="5">
-        <f>D13*E13</f>
-        <v>3.4999999999999996</v>
-      </c>
-    </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.35">
+        <f t="shared" si="0"/>
+        <v>1.1254019292604502</v>
+      </c>
+      <c r="F13" s="12">
+        <f t="shared" si="1"/>
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B14" s="2">
         <v>4</v>
       </c>
@@ -598,18 +601,18 @@
         <v>4.04</v>
       </c>
       <c r="D14" s="2">
-        <v>3.6</v>
+        <v>3.48</v>
       </c>
       <c r="E14" s="4">
-        <f>B14/D14</f>
-        <v>1.1111111111111112</v>
-      </c>
-      <c r="F14" s="5">
-        <f>D14*E14</f>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.35">
+        <f t="shared" si="0"/>
+        <v>1.1494252873563218</v>
+      </c>
+      <c r="F14" s="12">
+        <f t="shared" si="1"/>
+        <v>3.9999999999999996</v>
+      </c>
+    </row>
+    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B15" s="2">
         <v>4.5</v>
       </c>
@@ -617,18 +620,18 @@
         <v>4.5</v>
       </c>
       <c r="D15" s="2">
-        <v>4</v>
+        <v>3.95</v>
       </c>
       <c r="E15" s="4">
-        <f>B15/D15</f>
-        <v>1.125</v>
-      </c>
-      <c r="F15" s="5">
-        <f>D15*E15</f>
+        <f t="shared" si="0"/>
+        <v>1.1392405063291138</v>
+      </c>
+      <c r="F15" s="12">
+        <f t="shared" si="1"/>
         <v>4.5</v>
       </c>
     </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B16" s="2">
         <v>5</v>
       </c>
@@ -636,18 +639,18 @@
         <v>5</v>
       </c>
       <c r="D16" s="2">
-        <v>4.5199999999999996</v>
+        <v>4.43</v>
       </c>
       <c r="E16" s="4">
-        <f>B16/D16</f>
-        <v>1.1061946902654869</v>
-      </c>
-      <c r="F16" s="5">
-        <f>D16*E16</f>
+        <f t="shared" si="0"/>
+        <v>1.1286681715575622</v>
+      </c>
+      <c r="F16" s="12">
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B17" s="2">
         <v>5.5</v>
       </c>
@@ -655,18 +658,18 @@
         <v>5.45</v>
       </c>
       <c r="D17" s="2">
-        <v>4.93</v>
+        <v>5.09</v>
       </c>
       <c r="E17" s="4">
-        <f>B17/D17</f>
-        <v>1.1156186612576064</v>
-      </c>
-      <c r="F17" s="5">
-        <f>D17*E17</f>
-        <v>5.4999999999999991</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
+        <f t="shared" si="0"/>
+        <v>1.0805500982318272</v>
+      </c>
+      <c r="F17" s="12">
+        <f t="shared" si="1"/>
+        <v>5.5000000000000009</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B18" s="2">
         <v>6</v>
       </c>
@@ -674,18 +677,18 @@
         <v>5.9</v>
       </c>
       <c r="D18" s="2">
-        <v>5.5</v>
+        <v>5.59</v>
       </c>
       <c r="E18" s="4">
-        <f>B18/D18</f>
-        <v>1.0909090909090908</v>
-      </c>
-      <c r="F18" s="5">
-        <f>D18*E18</f>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
+        <f t="shared" si="0"/>
+        <v>1.0733452593917709</v>
+      </c>
+      <c r="F18" s="12">
+        <f t="shared" si="1"/>
+        <v>5.9999999999999991</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B19" s="2">
         <v>6.5</v>
       </c>
@@ -693,18 +696,18 @@
         <v>6.4</v>
       </c>
       <c r="D19" s="2">
-        <v>6.06</v>
+        <v>6.24</v>
       </c>
       <c r="E19" s="4">
-        <f>B19/D19</f>
-        <v>1.0726072607260726</v>
-      </c>
-      <c r="F19" s="5">
-        <f>D19*E19</f>
-        <v>6.4999999999999991</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
+        <f t="shared" si="0"/>
+        <v>1.0416666666666667</v>
+      </c>
+      <c r="F19" s="12">
+        <f t="shared" si="1"/>
+        <v>6.5000000000000009</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B20" s="2">
         <v>7</v>
       </c>
@@ -712,18 +715,18 @@
         <v>6.9</v>
       </c>
       <c r="D20" s="2">
-        <v>6.57</v>
+        <v>6.75</v>
       </c>
       <c r="E20" s="4">
-        <f>B20/D20</f>
-        <v>1.06544901065449</v>
-      </c>
-      <c r="F20" s="5">
-        <f>D20*E20</f>
+        <f t="shared" si="0"/>
+        <v>1.037037037037037</v>
+      </c>
+      <c r="F20" s="12">
+        <f t="shared" si="1"/>
         <v>7</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B21" s="2">
         <v>7.5</v>
       </c>
@@ -731,18 +734,18 @@
         <v>7.39</v>
       </c>
       <c r="D21" s="2">
-        <v>7.28</v>
+        <v>7.39</v>
       </c>
       <c r="E21" s="4">
-        <f>B21/D21</f>
-        <v>1.0302197802197801</v>
-      </c>
-      <c r="F21" s="5">
-        <f>D21*E21</f>
-        <v>7.4999999999999991</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
+        <f t="shared" si="0"/>
+        <v>1.0148849797023005</v>
+      </c>
+      <c r="F21" s="12">
+        <f t="shared" si="1"/>
+        <v>7.5000000000000009</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="7"/>
       <c r="B22" s="2">
         <v>8</v>
@@ -751,19 +754,19 @@
         <v>7.85</v>
       </c>
       <c r="D22" s="8">
-        <v>7.67</v>
+        <v>8.06</v>
       </c>
       <c r="E22" s="9">
-        <f>B22/D22</f>
-        <v>1.0430247718383312</v>
-      </c>
-      <c r="F22" s="10">
-        <f>D22*E22</f>
+        <f t="shared" si="0"/>
+        <v>0.99255583126550861</v>
+      </c>
+      <c r="F22" s="13">
+        <f t="shared" si="1"/>
         <v>8</v>
       </c>
       <c r="G22" s="10"/>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B23" s="2">
         <v>8.5</v>
       </c>
@@ -771,18 +774,18 @@
         <v>8.3000000000000007</v>
       </c>
       <c r="D23" s="2">
-        <v>8.31</v>
+        <v>8.7100000000000009</v>
       </c>
       <c r="E23" s="4">
-        <f>B23/D23</f>
-        <v>1.0228640192539109</v>
-      </c>
-      <c r="F23" s="5">
-        <f>D23*E23</f>
+        <f t="shared" si="0"/>
+        <v>0.97588978185993103</v>
+      </c>
+      <c r="F23" s="12">
+        <f t="shared" si="1"/>
         <v>8.5</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B24" s="2">
         <v>9</v>
       </c>
@@ -790,18 +793,18 @@
         <v>8.8000000000000007</v>
       </c>
       <c r="D24" s="2">
-        <v>8.84</v>
+        <v>9.2100000000000009</v>
       </c>
       <c r="E24" s="4">
-        <f>B24/D24</f>
-        <v>1.0180995475113122</v>
-      </c>
-      <c r="F24" s="5">
-        <f>D24*E24</f>
+        <f t="shared" si="0"/>
+        <v>0.97719869706840379</v>
+      </c>
+      <c r="F24" s="12">
+        <f t="shared" si="1"/>
         <v>9</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B25" s="2">
         <v>9.5</v>
       </c>
@@ -809,18 +812,18 @@
         <v>9.25</v>
       </c>
       <c r="D25" s="2">
-        <v>9.51</v>
+        <v>9.91</v>
       </c>
       <c r="E25" s="4">
-        <f>B25/D25</f>
-        <v>0.9989484752891693</v>
-      </c>
-      <c r="F25" s="5">
-        <f>D25*E25</f>
+        <f t="shared" si="0"/>
+        <v>0.95862764883955598</v>
+      </c>
+      <c r="F25" s="12">
+        <f t="shared" si="1"/>
         <v>9.5</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B26" s="2">
         <v>10</v>
       </c>
@@ -831,15 +834,15 @@
         <v>9.98</v>
       </c>
       <c r="E26" s="4">
-        <f>B26/D26</f>
+        <f t="shared" si="0"/>
         <v>1.002004008016032</v>
       </c>
-      <c r="F26" s="5">
-        <f>D26*E26</f>
+      <c r="F26" s="12">
+        <f t="shared" si="1"/>
         <v>10</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B27" s="2">
         <v>10.5</v>
       </c>
@@ -850,15 +853,15 @@
         <v>10.71</v>
       </c>
       <c r="E27" s="4">
-        <f>B27/D27</f>
+        <f t="shared" si="0"/>
         <v>0.98039215686274506</v>
       </c>
-      <c r="F27" s="5">
-        <f>D27*E27</f>
+      <c r="F27" s="12">
+        <f t="shared" si="1"/>
         <v>10.5</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B28" s="2">
         <v>11</v>
       </c>
@@ -869,19 +872,19 @@
         <v>11.22</v>
       </c>
       <c r="E28" s="4">
-        <f>B28/D28</f>
+        <f t="shared" si="0"/>
         <v>0.98039215686274506</v>
       </c>
-      <c r="F28" s="5">
-        <f>D28*E28</f>
+      <c r="F28" s="12">
+        <f t="shared" si="1"/>
         <v>11</v>
       </c>
       <c r="H28" s="6">
-        <f>D28-D27</f>
+        <f t="shared" ref="H28:H35" si="2">D28-D27</f>
         <v>0.50999999999999979</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B29" s="2">
         <v>11.5</v>
       </c>
@@ -892,19 +895,19 @@
         <v>11.82</v>
       </c>
       <c r="E29" s="4">
-        <f>B29/D29</f>
+        <f t="shared" si="0"/>
         <v>0.97292724196277491</v>
       </c>
-      <c r="F29" s="5">
-        <f>D29*E29</f>
+      <c r="F29" s="12">
+        <f t="shared" si="1"/>
         <v>11.5</v>
       </c>
       <c r="H29" s="6">
-        <f>D29-D28</f>
+        <f t="shared" si="2"/>
         <v>0.59999999999999964</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B30" s="2">
         <v>12</v>
       </c>
@@ -915,19 +918,19 @@
         <v>12.31</v>
       </c>
       <c r="E30" s="4">
-        <f>B30/D30</f>
+        <f t="shared" si="0"/>
         <v>0.9748172217709179</v>
       </c>
-      <c r="F30" s="5">
-        <f>D30*E30</f>
+      <c r="F30" s="12">
+        <f t="shared" si="1"/>
         <v>12</v>
       </c>
       <c r="H30" s="6">
-        <f>D30-D29</f>
+        <f t="shared" si="2"/>
         <v>0.49000000000000021</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B31" s="2">
         <v>12.5</v>
       </c>
@@ -938,19 +941,19 @@
         <v>13.15</v>
       </c>
       <c r="E31" s="4">
-        <f>B31/D31</f>
+        <f t="shared" si="0"/>
         <v>0.95057034220532322</v>
       </c>
-      <c r="F31" s="5">
-        <f>D31*E31</f>
+      <c r="F31" s="12">
+        <f t="shared" si="1"/>
         <v>12.5</v>
       </c>
       <c r="H31" s="6">
-        <f>D31-D30</f>
+        <f t="shared" si="2"/>
         <v>0.83999999999999986</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B32" s="2">
         <v>13</v>
       </c>
@@ -961,19 +964,19 @@
         <v>13.75</v>
       </c>
       <c r="E32" s="4">
-        <f>B32/D32</f>
+        <f t="shared" si="0"/>
         <v>0.94545454545454544</v>
       </c>
-      <c r="F32" s="5">
-        <f>D32*E32</f>
+      <c r="F32" s="12">
+        <f t="shared" si="1"/>
         <v>13</v>
       </c>
       <c r="H32" s="6">
-        <f>D32-D31</f>
+        <f t="shared" si="2"/>
         <v>0.59999999999999964</v>
       </c>
     </row>
-    <row r="33" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="33" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B33" s="2">
         <v>13.5</v>
       </c>
@@ -984,19 +987,19 @@
         <v>14.11</v>
       </c>
       <c r="E33" s="4">
-        <f>B33/D33</f>
+        <f t="shared" si="0"/>
         <v>0.95676824946846217</v>
       </c>
-      <c r="F33" s="5">
-        <f>D33*E33</f>
+      <c r="F33" s="12">
+        <f t="shared" si="1"/>
         <v>13.5</v>
       </c>
       <c r="H33" s="6">
-        <f>D33-D32</f>
+        <f t="shared" si="2"/>
         <v>0.35999999999999943</v>
       </c>
     </row>
-    <row r="34" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="34" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B34" s="2">
         <v>14</v>
       </c>
@@ -1007,19 +1010,19 @@
         <v>14.86</v>
       </c>
       <c r="E34" s="4">
-        <f>B34/D34</f>
+        <f t="shared" si="0"/>
         <v>0.94212651413189774</v>
       </c>
-      <c r="F34" s="5">
-        <f>D34*E34</f>
+      <c r="F34" s="12">
+        <f t="shared" si="1"/>
         <v>14</v>
       </c>
       <c r="H34" s="6">
-        <f>D34-D33</f>
+        <f t="shared" si="2"/>
         <v>0.75</v>
       </c>
     </row>
-    <row r="35" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="35" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B35" s="2">
         <v>14.5</v>
       </c>
@@ -1027,169 +1030,169 @@
         <v>8</v>
       </c>
       <c r="E35" s="4" t="e">
-        <f>B35/D35</f>
+        <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="F35" s="5" t="e">
-        <f>D35*E35</f>
+      <c r="F35" s="12" t="e">
+        <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
       <c r="H35" s="6">
-        <f>D35-D34</f>
+        <f t="shared" si="2"/>
         <v>-14.86</v>
       </c>
     </row>
-    <row r="36" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="36" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B36" s="2">
         <v>15</v>
       </c>
     </row>
-    <row r="37" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="37" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B37" s="2">
         <v>15.5</v>
       </c>
     </row>
-    <row r="38" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="38" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B38" s="2">
         <v>16</v>
       </c>
     </row>
-    <row r="39" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="39" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B39" s="2">
         <v>16.5</v>
       </c>
     </row>
-    <row r="40" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="40" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B40" s="2">
         <v>17</v>
       </c>
     </row>
-    <row r="41" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="41" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B41" s="2">
         <v>17.5</v>
       </c>
     </row>
-    <row r="42" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="42" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B42" s="2">
         <v>18</v>
       </c>
     </row>
-    <row r="43" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="43" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B43" s="2">
         <v>18.5</v>
       </c>
     </row>
-    <row r="44" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="44" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B44" s="2">
         <v>19</v>
       </c>
     </row>
-    <row r="45" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="45" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B45" s="2">
         <v>19.5</v>
       </c>
     </row>
-    <row r="46" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="46" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B46" s="2">
         <v>20</v>
       </c>
     </row>
-    <row r="47" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="47" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B47" s="2">
         <v>20.5</v>
       </c>
     </row>
-    <row r="48" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="48" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B48" s="2">
         <v>21</v>
       </c>
     </row>
-    <row r="49" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="49" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B49" s="2">
         <v>21.5</v>
       </c>
     </row>
-    <row r="50" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="50" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B50" s="2">
         <v>22</v>
       </c>
     </row>
-    <row r="51" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="51" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B51" s="2">
         <v>22.5</v>
       </c>
     </row>
-    <row r="52" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="52" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B52" s="2">
         <v>23</v>
       </c>
     </row>
-    <row r="53" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="53" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B53" s="2">
         <v>23.5</v>
       </c>
     </row>
-    <row r="54" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="54" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B54" s="2">
         <v>24</v>
       </c>
     </row>
-    <row r="55" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="55" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B55" s="2">
         <v>24.5</v>
       </c>
     </row>
-    <row r="56" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="56" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B56" s="2">
         <v>25</v>
       </c>
     </row>
-    <row r="57" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="57" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B57" s="2">
         <v>25.5</v>
       </c>
     </row>
-    <row r="58" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="58" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B58" s="2">
         <v>26</v>
       </c>
     </row>
-    <row r="59" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="59" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B59" s="2">
         <v>26.5</v>
       </c>
     </row>
-    <row r="60" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="60" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B60" s="2">
         <v>27</v>
       </c>
     </row>
-    <row r="61" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="61" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B61" s="2">
         <v>27.5</v>
       </c>
     </row>
-    <row r="62" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="62" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B62" s="2">
         <v>28</v>
       </c>
     </row>
-    <row r="63" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="63" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B63" s="2">
         <v>28.5</v>
       </c>
     </row>
-    <row r="64" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="64" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B64" s="2">
         <v>29</v>
       </c>
     </row>
-    <row r="65" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="65" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B65" s="2">
         <v>29.5</v>
       </c>
     </row>
-    <row r="66" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="66" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B66" s="2">
         <v>30</v>
       </c>
@@ -1209,6 +1212,12 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="14.28515625" customWidth="1"/>
+    <col min="3" max="3" width="15.140625" customWidth="1"/>
+    <col min="4" max="4" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.42578125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B1" t="s">

</xml_diff>

<commit_message>
current calculation done as per ruquired
current calculation done as per required
</commit_message>
<xml_diff>
--- a/cureent table.xlsx
+++ b/cureent table.xlsx
@@ -427,8 +427,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A6:H66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -471,11 +471,11 @@
         <v>0.5</v>
       </c>
       <c r="E7" s="4">
-        <f t="shared" ref="E7:E35" si="0">B7/D7</f>
+        <f t="shared" ref="E7:E45" si="0">B7/D7</f>
         <v>1</v>
       </c>
       <c r="F7" s="12">
-        <f t="shared" ref="F7:F35" si="1">D7*E7</f>
+        <f t="shared" ref="F7:F45" si="1">D7*E7</f>
         <v>0.5</v>
       </c>
     </row>
@@ -487,11 +487,11 @@
         <v>1.1100000000000001</v>
       </c>
       <c r="D8" s="2">
-        <v>0.99</v>
+        <v>0.97</v>
       </c>
       <c r="E8" s="4">
         <f t="shared" si="0"/>
-        <v>1.0101010101010102</v>
+        <v>1.0309278350515465</v>
       </c>
       <c r="F8" s="12">
         <f>D8*E8</f>
@@ -506,11 +506,11 @@
         <v>1.61</v>
       </c>
       <c r="D9" s="2">
-        <v>1.32</v>
+        <v>1.24</v>
       </c>
       <c r="E9" s="4">
         <f t="shared" si="0"/>
-        <v>1.1363636363636362</v>
+        <v>1.2096774193548387</v>
       </c>
       <c r="F9" s="12">
         <f t="shared" si="1"/>
@@ -525,11 +525,11 @@
         <v>2.06</v>
       </c>
       <c r="D10" s="2">
-        <v>1.81</v>
+        <v>1.7</v>
       </c>
       <c r="E10" s="4">
         <f t="shared" si="0"/>
-        <v>1.1049723756906078</v>
+        <v>1.1764705882352942</v>
       </c>
       <c r="F10" s="12">
         <f t="shared" si="1"/>
@@ -544,11 +544,11 @@
         <v>2.56</v>
       </c>
       <c r="D11" s="2">
-        <v>2.14</v>
+        <v>2.06</v>
       </c>
       <c r="E11" s="4">
         <f t="shared" si="0"/>
-        <v>1.1682242990654206</v>
+        <v>1.2135922330097086</v>
       </c>
       <c r="F11" s="12">
         <f t="shared" si="1"/>
@@ -563,11 +563,11 @@
         <v>3.01</v>
       </c>
       <c r="D12" s="2">
-        <v>2.63</v>
+        <v>2.52</v>
       </c>
       <c r="E12" s="4">
         <f t="shared" si="0"/>
-        <v>1.1406844106463878</v>
+        <v>1.1904761904761905</v>
       </c>
       <c r="F12" s="12">
         <f t="shared" si="1"/>
@@ -582,11 +582,11 @@
         <v>3.51</v>
       </c>
       <c r="D13" s="2">
-        <v>3.11</v>
+        <v>2.9</v>
       </c>
       <c r="E13" s="4">
         <f t="shared" si="0"/>
-        <v>1.1254019292604502</v>
+        <v>1.2068965517241379</v>
       </c>
       <c r="F13" s="12">
         <f t="shared" si="1"/>
@@ -601,11 +601,11 @@
         <v>4.04</v>
       </c>
       <c r="D14" s="2">
-        <v>3.48</v>
+        <v>3.28</v>
       </c>
       <c r="E14" s="4">
         <f t="shared" si="0"/>
-        <v>1.1494252873563218</v>
+        <v>1.2195121951219512</v>
       </c>
       <c r="F14" s="12">
         <f t="shared" si="1"/>
@@ -620,11 +620,11 @@
         <v>4.5</v>
       </c>
       <c r="D15" s="2">
-        <v>3.95</v>
+        <v>3.85</v>
       </c>
       <c r="E15" s="4">
         <f t="shared" si="0"/>
-        <v>1.1392405063291138</v>
+        <v>1.1688311688311688</v>
       </c>
       <c r="F15" s="12">
         <f t="shared" si="1"/>
@@ -639,11 +639,11 @@
         <v>5</v>
       </c>
       <c r="D16" s="2">
-        <v>4.43</v>
+        <v>4.3600000000000003</v>
       </c>
       <c r="E16" s="4">
         <f t="shared" si="0"/>
-        <v>1.1286681715575622</v>
+        <v>1.1467889908256881</v>
       </c>
       <c r="F16" s="12">
         <f t="shared" si="1"/>
@@ -658,15 +658,15 @@
         <v>5.45</v>
       </c>
       <c r="D17" s="2">
-        <v>5.09</v>
+        <v>4.88</v>
       </c>
       <c r="E17" s="4">
         <f t="shared" si="0"/>
-        <v>1.0805500982318272</v>
+        <v>1.1270491803278688</v>
       </c>
       <c r="F17" s="12">
         <f t="shared" si="1"/>
-        <v>5.5000000000000009</v>
+        <v>5.5</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
@@ -677,15 +677,15 @@
         <v>5.9</v>
       </c>
       <c r="D18" s="2">
-        <v>5.59</v>
+        <v>5.33</v>
       </c>
       <c r="E18" s="4">
         <f t="shared" si="0"/>
-        <v>1.0733452593917709</v>
+        <v>1.125703564727955</v>
       </c>
       <c r="F18" s="12">
         <f t="shared" si="1"/>
-        <v>5.9999999999999991</v>
+        <v>6</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
@@ -696,15 +696,15 @@
         <v>6.4</v>
       </c>
       <c r="D19" s="2">
-        <v>6.24</v>
+        <v>5.83</v>
       </c>
       <c r="E19" s="4">
         <f t="shared" si="0"/>
-        <v>1.0416666666666667</v>
+        <v>1.1149228130360205</v>
       </c>
       <c r="F19" s="12">
         <f t="shared" si="1"/>
-        <v>6.5000000000000009</v>
+        <v>6.4999999999999991</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
@@ -715,15 +715,15 @@
         <v>6.9</v>
       </c>
       <c r="D20" s="2">
-        <v>6.75</v>
+        <v>6.47</v>
       </c>
       <c r="E20" s="4">
         <f t="shared" si="0"/>
-        <v>1.037037037037037</v>
+        <v>1.081916537867079</v>
       </c>
       <c r="F20" s="12">
         <f t="shared" si="1"/>
-        <v>7</v>
+        <v>7.0000000000000009</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
@@ -734,15 +734,15 @@
         <v>7.39</v>
       </c>
       <c r="D21" s="2">
-        <v>7.39</v>
+        <v>6.92</v>
       </c>
       <c r="E21" s="4">
         <f t="shared" si="0"/>
-        <v>1.0148849797023005</v>
+        <v>1.0838150289017341</v>
       </c>
       <c r="F21" s="12">
         <f t="shared" si="1"/>
-        <v>7.5000000000000009</v>
+        <v>7.5</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
@@ -754,11 +754,11 @@
         <v>7.85</v>
       </c>
       <c r="D22" s="8">
-        <v>8.06</v>
+        <v>7.51</v>
       </c>
       <c r="E22" s="9">
         <f t="shared" si="0"/>
-        <v>0.99255583126550861</v>
+        <v>1.0652463382157125</v>
       </c>
       <c r="F22" s="13">
         <f t="shared" si="1"/>
@@ -774,11 +774,11 @@
         <v>8.3000000000000007</v>
       </c>
       <c r="D23" s="2">
-        <v>8.7100000000000009</v>
+        <v>8.01</v>
       </c>
       <c r="E23" s="4">
         <f t="shared" si="0"/>
-        <v>0.97588978185993103</v>
+        <v>1.0611735330836454</v>
       </c>
       <c r="F23" s="12">
         <f t="shared" si="1"/>
@@ -793,11 +793,11 @@
         <v>8.8000000000000007</v>
       </c>
       <c r="D24" s="2">
-        <v>9.2100000000000009</v>
+        <v>8.76</v>
       </c>
       <c r="E24" s="4">
         <f t="shared" si="0"/>
-        <v>0.97719869706840379</v>
+        <v>1.0273972602739727</v>
       </c>
       <c r="F24" s="12">
         <f t="shared" si="1"/>
@@ -812,11 +812,11 @@
         <v>9.25</v>
       </c>
       <c r="D25" s="2">
-        <v>9.91</v>
+        <v>9.27</v>
       </c>
       <c r="E25" s="4">
         <f t="shared" si="0"/>
-        <v>0.95862764883955598</v>
+        <v>1.0248112189859764</v>
       </c>
       <c r="F25" s="12">
         <f t="shared" si="1"/>
@@ -831,11 +831,11 @@
         <v>9.7899999999999991</v>
       </c>
       <c r="D26" s="2">
-        <v>9.98</v>
+        <v>10</v>
       </c>
       <c r="E26" s="4">
         <f t="shared" si="0"/>
-        <v>1.002004008016032</v>
+        <v>1</v>
       </c>
       <c r="F26" s="12">
         <f t="shared" si="1"/>
@@ -850,11 +850,11 @@
         <v>10.24</v>
       </c>
       <c r="D27" s="2">
-        <v>10.71</v>
+        <v>10.42</v>
       </c>
       <c r="E27" s="4">
         <f t="shared" si="0"/>
-        <v>0.98039215686274506</v>
+        <v>1.0076775431861804</v>
       </c>
       <c r="F27" s="12">
         <f t="shared" si="1"/>
@@ -869,11 +869,11 @@
         <v>10.74</v>
       </c>
       <c r="D28" s="2">
-        <v>11.22</v>
+        <v>10.96</v>
       </c>
       <c r="E28" s="4">
         <f t="shared" si="0"/>
-        <v>0.98039215686274506</v>
+        <v>1.0036496350364963</v>
       </c>
       <c r="F28" s="12">
         <f t="shared" si="1"/>
@@ -881,7 +881,7 @@
       </c>
       <c r="H28" s="6">
         <f t="shared" ref="H28:H35" si="2">D28-D27</f>
-        <v>0.50999999999999979</v>
+        <v>0.54000000000000092</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
@@ -892,11 +892,11 @@
         <v>11.19</v>
       </c>
       <c r="D29" s="2">
-        <v>11.82</v>
+        <v>11.51</v>
       </c>
       <c r="E29" s="4">
         <f t="shared" si="0"/>
-        <v>0.97292724196277491</v>
+        <v>0.99913119026933106</v>
       </c>
       <c r="F29" s="12">
         <f t="shared" si="1"/>
@@ -904,7 +904,7 @@
       </c>
       <c r="H29" s="6">
         <f t="shared" si="2"/>
-        <v>0.59999999999999964</v>
+        <v>0.54999999999999893</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
@@ -915,11 +915,11 @@
         <v>11.65</v>
       </c>
       <c r="D30" s="2">
-        <v>12.31</v>
+        <v>12.04</v>
       </c>
       <c r="E30" s="4">
         <f t="shared" si="0"/>
-        <v>0.9748172217709179</v>
+        <v>0.99667774086378746</v>
       </c>
       <c r="F30" s="12">
         <f t="shared" si="1"/>
@@ -927,7 +927,7 @@
       </c>
       <c r="H30" s="6">
         <f t="shared" si="2"/>
-        <v>0.49000000000000021</v>
+        <v>0.52999999999999936</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
@@ -938,11 +938,11 @@
         <v>12.19</v>
       </c>
       <c r="D31" s="11">
-        <v>13.15</v>
+        <v>12.69</v>
       </c>
       <c r="E31" s="4">
         <f t="shared" si="0"/>
-        <v>0.95057034220532322</v>
+        <v>0.98502758077226171</v>
       </c>
       <c r="F31" s="12">
         <f t="shared" si="1"/>
@@ -950,7 +950,7 @@
       </c>
       <c r="H31" s="6">
         <f t="shared" si="2"/>
-        <v>0.83999999999999986</v>
+        <v>0.65000000000000036</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
@@ -961,11 +961,11 @@
         <v>12.68</v>
       </c>
       <c r="D32" s="2">
-        <v>13.75</v>
+        <v>13.14</v>
       </c>
       <c r="E32" s="4">
         <f t="shared" si="0"/>
-        <v>0.94545454545454544</v>
+        <v>0.98934550989345504</v>
       </c>
       <c r="F32" s="12">
         <f t="shared" si="1"/>
@@ -973,7 +973,7 @@
       </c>
       <c r="H32" s="6">
         <f t="shared" si="2"/>
-        <v>0.59999999999999964</v>
+        <v>0.45000000000000107</v>
       </c>
     </row>
     <row r="33" spans="2:8" x14ac:dyDescent="0.25">
@@ -984,11 +984,11 @@
         <v>13.14</v>
       </c>
       <c r="D33" s="2">
-        <v>14.11</v>
+        <v>13.8</v>
       </c>
       <c r="E33" s="4">
         <f t="shared" si="0"/>
-        <v>0.95676824946846217</v>
+        <v>0.97826086956521729</v>
       </c>
       <c r="F33" s="12">
         <f t="shared" si="1"/>
@@ -996,7 +996,7 @@
       </c>
       <c r="H33" s="6">
         <f t="shared" si="2"/>
-        <v>0.35999999999999943</v>
+        <v>0.66000000000000014</v>
       </c>
     </row>
     <row r="34" spans="2:8" x14ac:dyDescent="0.25">
@@ -1007,11 +1007,11 @@
         <v>13.63</v>
       </c>
       <c r="D34" s="2">
-        <v>14.86</v>
+        <v>14.32</v>
       </c>
       <c r="E34" s="4">
         <f t="shared" si="0"/>
-        <v>0.94212651413189774</v>
+        <v>0.97765363128491622</v>
       </c>
       <c r="F34" s="12">
         <f t="shared" si="1"/>
@@ -1019,7 +1019,7 @@
       </c>
       <c r="H34" s="6">
         <f t="shared" si="2"/>
-        <v>0.75</v>
+        <v>0.51999999999999957</v>
       </c>
     </row>
     <row r="35" spans="2:8" x14ac:dyDescent="0.25">
@@ -1029,76 +1029,211 @@
       <c r="C35" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E35" s="4" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F35" s="12" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+      <c r="D35" s="2">
+        <v>14.96</v>
+      </c>
+      <c r="E35" s="4">
+        <f t="shared" si="0"/>
+        <v>0.96925133689839571</v>
+      </c>
+      <c r="F35" s="12">
+        <f t="shared" si="1"/>
+        <v>14.5</v>
       </c>
       <c r="H35" s="6">
         <f t="shared" si="2"/>
-        <v>-14.86</v>
+        <v>0.64000000000000057</v>
       </c>
     </row>
     <row r="36" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B36" s="2">
         <v>15</v>
       </c>
+      <c r="D36" s="2">
+        <v>15.43</v>
+      </c>
+      <c r="E36" s="4">
+        <f t="shared" si="0"/>
+        <v>0.97213220998055738</v>
+      </c>
+      <c r="F36" s="12">
+        <f t="shared" si="1"/>
+        <v>15</v>
+      </c>
     </row>
     <row r="37" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B37" s="2">
         <v>15.5</v>
       </c>
+      <c r="D37" s="2">
+        <v>16.04</v>
+      </c>
+      <c r="E37" s="4">
+        <f t="shared" si="0"/>
+        <v>0.96633416458852872</v>
+      </c>
+      <c r="F37" s="12">
+        <f t="shared" si="1"/>
+        <v>15.5</v>
+      </c>
     </row>
     <row r="38" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B38" s="2">
         <v>16</v>
       </c>
+      <c r="D38" s="2">
+        <v>16.61</v>
+      </c>
+      <c r="E38" s="4">
+        <f t="shared" si="0"/>
+        <v>0.96327513546056598</v>
+      </c>
+      <c r="F38" s="12">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
     </row>
     <row r="39" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B39" s="2">
         <v>16.5</v>
       </c>
+      <c r="D39" s="2">
+        <v>17.09</v>
+      </c>
+      <c r="E39" s="4">
+        <f t="shared" si="0"/>
+        <v>0.96547688706846113</v>
+      </c>
+      <c r="F39" s="12">
+        <f t="shared" si="1"/>
+        <v>16.5</v>
+      </c>
     </row>
     <row r="40" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B40" s="2">
         <v>17</v>
       </c>
+      <c r="D40" s="2">
+        <v>17.690000000000001</v>
+      </c>
+      <c r="E40" s="4">
+        <f t="shared" si="0"/>
+        <v>0.96099491237987555</v>
+      </c>
+      <c r="F40" s="12">
+        <f t="shared" si="1"/>
+        <v>17</v>
+      </c>
     </row>
     <row r="41" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B41" s="2">
         <v>17.5</v>
       </c>
+      <c r="D41" s="2">
+        <v>18.170000000000002</v>
+      </c>
+      <c r="E41" s="4">
+        <f t="shared" si="0"/>
+        <v>0.96312603192074842</v>
+      </c>
+      <c r="F41" s="12">
+        <f t="shared" si="1"/>
+        <v>17.5</v>
+      </c>
     </row>
     <row r="42" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B42" s="2">
         <v>18</v>
       </c>
+      <c r="D42" s="2">
+        <v>18.78</v>
+      </c>
+      <c r="E42" s="4">
+        <f t="shared" si="0"/>
+        <v>0.95846645367412131</v>
+      </c>
+      <c r="F42" s="12">
+        <f t="shared" si="1"/>
+        <v>18</v>
+      </c>
     </row>
     <row r="43" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B43" s="2">
         <v>18.5</v>
       </c>
+      <c r="D43" s="2">
+        <v>19.29</v>
+      </c>
+      <c r="E43" s="4">
+        <f t="shared" si="0"/>
+        <v>0.95904613789528259</v>
+      </c>
+      <c r="F43" s="12">
+        <f t="shared" si="1"/>
+        <v>18.5</v>
+      </c>
     </row>
     <row r="44" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B44" s="2">
         <v>19</v>
       </c>
+      <c r="D44" s="2">
+        <v>19.79</v>
+      </c>
+      <c r="E44" s="4">
+        <f t="shared" si="0"/>
+        <v>0.9600808489135928</v>
+      </c>
+      <c r="F44" s="12">
+        <f t="shared" si="1"/>
+        <v>19</v>
+      </c>
     </row>
     <row r="45" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B45" s="2">
         <v>19.5</v>
       </c>
+      <c r="D45" s="2">
+        <v>20.63</v>
+      </c>
+      <c r="E45" s="4">
+        <f t="shared" si="0"/>
+        <v>0.94522539990305388</v>
+      </c>
+      <c r="F45" s="12">
+        <f t="shared" si="1"/>
+        <v>19.5</v>
+      </c>
     </row>
     <row r="46" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B46" s="2">
         <v>20</v>
       </c>
+      <c r="D46" s="2">
+        <v>21.23</v>
+      </c>
+      <c r="E46" s="4">
+        <f t="shared" ref="E46:E47" si="3">B46/D46</f>
+        <v>0.9420631182289213</v>
+      </c>
+      <c r="F46" s="12">
+        <f t="shared" ref="F46:F47" si="4">D46*E46</f>
+        <v>20</v>
+      </c>
     </row>
     <row r="47" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B47" s="2">
+        <v>20.5</v>
+      </c>
+      <c r="D47" s="2">
+        <v>21.92</v>
+      </c>
+      <c r="E47" s="4">
+        <f t="shared" si="3"/>
+        <v>0.93521897810218968</v>
+      </c>
+      <c r="F47" s="12">
+        <f t="shared" si="4"/>
         <v>20.5</v>
       </c>
     </row>

</xml_diff>